<commit_message>
Fixed dataframes, added headers
Now writes out dataframes to excel workbooks. Puts 0.0 for missing fields.
</commit_message>
<xml_diff>
--- a/2018_data/Kyle_Allen2018.xlsx
+++ b/2018_data/Kyle_Allen2018.xlsx
@@ -345,293 +345,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC2"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Allen</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Kyle</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>QB</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>2018-12-23</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>22.290</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>CAR</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr"/>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>ATL</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>L 10-24</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr"/>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>100.00</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>38</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>106.2</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>9.50</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>9.50</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr"/>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AC1" t="n">
-        <v>1.52</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Allen</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Kyle</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>QB</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2018-12-30</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>22.297</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>CAR</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>NOR</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>W 33-14</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>*</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>59.26</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>228</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>111.3</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>8.44</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>9.93</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
-      </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>3.80</t>
-        </is>
-      </c>
-      <c r="Z2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AA2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AB2" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="AC2" t="n">
-        <v>25.02</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>